<commit_message>
Updated graph for max flow
</commit_message>
<xml_diff>
--- a/max_flow/mfGraph.xlsx
+++ b/max_flow/mfGraph.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documents\Independent Study\DistributedGraphProcessingSystem\mst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documents\Independent Study\DistributedGraphProcessingSystem\max_flow\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,24 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>1,8,4</t>
+    <t>1,8,4,-1</t>
   </si>
   <si>
-    <t>1,3,3</t>
+    <t>3,3</t>
   </si>
   <si>
-    <t>8,10,2</t>
-  </si>
-  <si>
-    <t>4,3,7</t>
-  </si>
-  <si>
-    <t>3,0</t>
-  </si>
-  <si>
-    <t>2,0</t>
+    <t>8,10</t>
   </si>
 </sst>
 </file>
@@ -397,7 +388,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,40 +426,34 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
+      <c r="B5">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="B6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
+      <c r="B9">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
@@ -478,17 +463,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -561,78 +546,6 @@
       </c>
       <c r="B10">
         <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>7</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>